<commit_message>
Jan 20 - Tier-2 brands update
</commit_message>
<xml_diff>
--- a/gr_optimization/Input_Output/BuyflowValidation/Merchandising Input/MeaningfulBeauty/mb5-deluxe20offb15.xlsx
+++ b/gr_optimization/Input_Output/BuyflowValidation/Merchandising Input/MeaningfulBeauty/mb5-deluxe20offb15.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23621"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23716"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{45B69825-15DC-42C4-9EA4-46FCE423647F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{159CD447-3633-4845-84CD-A84262827036}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{45B69825-15DC-42C4-9EA4-46FCE423647F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1A498563-2813-4AC0-81BC-373B22C526FF}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Active Campaign" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="185">
   <si>
     <t>Vanity URL</t>
   </si>
@@ -442,7 +442,7 @@
     <t>Pre-Purchase Entry Shipping</t>
   </si>
   <si>
-    <t>Pre-Purchase Entry Renewal Plan</t>
+    <t>Pre-Purchase Entry Renewal Plan</t>
   </si>
   <si>
     <t>RMTA4AD</t>
@@ -608,9 +608,6 @@
 • 1st Payment: $44.95 charged today (Free Standard S&amp;H)
 • 2nd Payment: $44.95 charged one month from today
 • 3rd Payment: $44.95 charged two months from today</t>
-  </si>
-  <si>
-    <t>Pre-Purchase Entry Renewal Plan</t>
   </si>
 </sst>
 </file>
@@ -1344,8 +1341,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2780,8 +2777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D964B158-45D0-4859-9DA3-995A04CCFEEE}">
   <dimension ref="A1:J97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3622,7 +3619,7 @@
     </row>
     <row r="62" spans="1:4" ht="15.75">
       <c r="A62" s="13" t="s">
-        <v>185</v>
+        <v>136</v>
       </c>
       <c r="B62" s="14" t="s">
         <v>137</v>
@@ -4105,15 +4102,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C47EEB8100460B478BDC3BCCBE3D5051" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="829e995fc61fbfa25718206016b29da6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c6a6306-8d4e-455f-a7d8-70154a0dc4d2" xmlns:ns3="3e63a3be-2d53-41f2-914e-dd0efc332534" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3545440ad2b936a9d10385f8b267d779" ns2:_="" ns3:_="">
     <xsd:import namespace="9c6a6306-8d4e-455f-a7d8-70154a0dc4d2"/>
@@ -4278,14 +4266,23 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86F5D631-A150-4668-A8EB-947DB3A2A4E8}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1889725-2C06-4DD3-B199-3839718C49C5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A187F77C-E3B1-4B81-88C3-5890496FD075}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A187F77C-E3B1-4B81-88C3-5890496FD075}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1889725-2C06-4DD3-B199-3839718C49C5}"/>
 </file>
</xml_diff>